<commit_message>
After meeting with Del
</commit_message>
<xml_diff>
--- a/docs/user_stories.xlsx
+++ b/docs/user_stories.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="188" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="188" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stories" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Questions" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="objects_and_attr" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -210,7 +211,163 @@
     <t>Should we just write the notes into a single view and do matching there instead of worrying about persisting in a database? Will it make it easier or harder to use regex?</t>
   </si>
   <si>
-    <t>resume </t>
+    <t>resume</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password_digest</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>tag_id</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>comment_id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>relates to: post, comment, story, feature, step?</t>
+  </si>
+  <si>
+    <t>user_roles</t>
+  </si>
+  <si>
+    <t>role_name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>looks like we should breakup the table differently if each row could only relate to a single user_id, story_id, feature_id</t>
+  </si>
+  <si>
+    <t>story_id</t>
+  </si>
+  <si>
+    <t>feature_id</t>
+  </si>
+  <si>
+    <t>feature_steps</t>
+  </si>
+  <si>
+    <t>used to sequence steps in a given feature</t>
+  </si>
+  <si>
+    <t>feature_step_number</t>
+  </si>
+  <si>
+    <t>item?</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>looks like we should breakup the table differently if each</t>
+  </si>
+  <si>
+    <t>commentable</t>
+  </si>
+  <si>
+    <t>commentable_type</t>
+  </si>
+  <si>
+    <t>rankings</t>
+  </si>
+  <si>
+    <t>should this be global or by story, feature, step?</t>
+  </si>
+  <si>
+    <t>avg_time</t>
+  </si>
+  <si>
+    <t>highscore</t>
+  </si>
+  <si>
+    <t>story</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>feature</t>
+  </si>
+  <si>
+    <t>feature_type</t>
+  </si>
+  <si>
+    <t>tags?</t>
+  </si>
+  <si>
+    <t>relates to tag( function/method, model, view, controller, class)</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>should we use to also group our “courses” together</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>(language, technology, skilllevel, framework.)</t>
+  </si>
+  <si>
+    <t>resources_helpful_links</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>type_of_resource</t>
+  </si>
+  <si>
+    <t>url, a video, blog post, etc.</t>
+  </si>
+  <si>
+    <t>story_feature</t>
   </si>
 </sst>
 </file>
@@ -225,6 +382,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -246,9 +404,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +418,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9900"/>
         <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -303,7 +468,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,6 +478,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,12 +500,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -1019,13 +1188,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1070,7 +1239,532 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:E55"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="95.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>